<commit_message>
altering create report functionality
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>Full Name</t>
   </si>
@@ -22,6 +22,15 @@
     <t>Username</t>
   </si>
   <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Last Login</t>
+  </si>
+  <si>
     <t>Abbas Ali Khalid</t>
   </si>
   <si>
@@ -37,6 +46,51 @@
     <t>Wellisama</t>
   </si>
   <si>
+    <t>khalid ali mazen</t>
+  </si>
+  <si>
+    <t>Ramy Ali Hassan</t>
+  </si>
+  <si>
+    <t>Julia Marple</t>
+  </si>
+  <si>
+    <t>Lamia Ali Salih</t>
+  </si>
+  <si>
+    <t>sohair ali khalid</t>
+  </si>
+  <si>
+    <t>waleed Mohammed Hassan</t>
+  </si>
+  <si>
+    <t>alaa</t>
+  </si>
+  <si>
+    <t>Ahmed Adel</t>
+  </si>
+  <si>
+    <t>Sami Adel</t>
+  </si>
+  <si>
+    <t>Ali Adel</t>
+  </si>
+  <si>
+    <t>Reham Adel</t>
+  </si>
+  <si>
+    <t>Alaa Adel</t>
+  </si>
+  <si>
+    <t>Samah Adel</t>
+  </si>
+  <si>
+    <t>Qassim Ahmed</t>
+  </si>
+  <si>
+    <t>Reham Salih</t>
+  </si>
+  <si>
     <t>Remaz Essam</t>
   </si>
   <si>
@@ -58,6 +112,45 @@
     <t>Samia</t>
   </si>
   <si>
+    <t>khalid</t>
+  </si>
+  <si>
+    <t>ramy</t>
+  </si>
+  <si>
+    <t>loly</t>
+  </si>
+  <si>
+    <t>somy</t>
+  </si>
+  <si>
+    <t>willi</t>
+  </si>
+  <si>
+    <t>ahmed23</t>
+  </si>
+  <si>
+    <t>Sami23</t>
+  </si>
+  <si>
+    <t>Ali23</t>
+  </si>
+  <si>
+    <t>Reham23</t>
+  </si>
+  <si>
+    <t>Alaa</t>
+  </si>
+  <si>
+    <t>Samah</t>
+  </si>
+  <si>
+    <t>samwa</t>
+  </si>
+  <si>
+    <t>rere</t>
+  </si>
+  <si>
     <t>Remaz</t>
   </si>
   <si>
@@ -65,6 +158,123 @@
   </si>
   <si>
     <t>fofa</t>
+  </si>
+  <si>
+    <t>Unisoft</t>
+  </si>
+  <si>
+    <t>Unigroup</t>
+  </si>
+  <si>
+    <t>UniSoft-SD</t>
+  </si>
+  <si>
+    <t>Unicom</t>
+  </si>
+  <si>
+    <t>unisoft</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>0111123211</t>
+  </si>
+  <si>
+    <t>0999865676</t>
+  </si>
+  <si>
+    <t>0983432123</t>
+  </si>
+  <si>
+    <t>0908779558</t>
+  </si>
+  <si>
+    <t>0127372724</t>
+  </si>
+  <si>
+    <t>0999232345</t>
+  </si>
+  <si>
+    <t>0923212345</t>
+  </si>
+  <si>
+    <t>0908775558</t>
+  </si>
+  <si>
+    <t>0987654003</t>
+  </si>
+  <si>
+    <t>0123234543</t>
+  </si>
+  <si>
+    <t>0122132300</t>
+  </si>
+  <si>
+    <t>0907046413</t>
+  </si>
+  <si>
+    <t>0913432120</t>
+  </si>
+  <si>
+    <t>0913430120</t>
+  </si>
+  <si>
+    <t>0113430120</t>
+  </si>
+  <si>
+    <t>0123430120</t>
+  </si>
+  <si>
+    <t>0923930120</t>
+  </si>
+  <si>
+    <t>0122900120</t>
+  </si>
+  <si>
+    <t>0999627378</t>
+  </si>
+  <si>
+    <t>0987332316</t>
+  </si>
+  <si>
+    <t>0987876543</t>
+  </si>
+  <si>
+    <t>0987705430</t>
+  </si>
+  <si>
+    <t>0920111214</t>
+  </si>
+  <si>
+    <t>0906856854</t>
+  </si>
+  <si>
+    <t>0909089895</t>
+  </si>
+  <si>
+    <t>02-08-21 Mon 19:24 PM</t>
+  </si>
+  <si>
+    <t>02-08-21 Mon 19:27 PM</t>
+  </si>
+  <si>
+    <t>02-08-21 Mon 19:25 PM</t>
+  </si>
+  <si>
+    <t>03-08-21 Tue 13:01 PM</t>
+  </si>
+  <si>
+    <t>22-08-21 Sun 06:50 AM</t>
+  </si>
+  <si>
+    <t>04-08-21 Wed 06:10 AM</t>
+  </si>
+  <si>
+    <t>16-08-21 Mon 08:17 AM</t>
+  </si>
+  <si>
+    <t>16-08-21 Mon 08:51 AM</t>
   </si>
 </sst>
 </file>
@@ -396,98 +606,449 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>